<commit_message>
Split between scheme name and issuing agency
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="351">
   <si>
     <t>GLN</t>
   </si>
@@ -131,9 +131,6 @@
     <t>EU:VAT</t>
   </si>
   <si>
-    <t>National ministries of Economy</t>
-  </si>
-  <si>
     <t>EU:REID</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
   </si>
   <si>
     <t>AT:CID</t>
-  </si>
-  <si>
-    <t>Firmenidentifikationsnummer der Statistik Austria</t>
   </si>
   <si>
     <t>IS:KT</t>
@@ -729,9 +723,6 @@
   </si>
   <si>
     <t>1.1.2</t>
-  </si>
-  <si>
-    <t>Vereniging van Kamers van Koophandel en Fabrieken in Nederland, Scheme</t>
   </si>
   <si>
     <t>9954</t>
@@ -907,10 +898,6 @@
     <t>0130</t>
   </si>
   <si>
-    <t>European Commission, Information Directorate, Data Transmission Service, Rue de
-la Loi, 200, B-1049 Brussels, Belgium</t>
-  </si>
-  <si>
     <t>1) ICD 4 digits, 2) None</t>
   </si>
   <si>
@@ -1077,6 +1064,73 @@
   </si>
   <si>
     <t>VA</t>
+  </si>
+  <si>
+    <t>System Information et Repertoire des Entreprise et des Etablissements: SIRENE</t>
+  </si>
+  <si>
+    <t>Organisationsnummer</t>
+  </si>
+  <si>
+    <t>SIRET-CODE</t>
+  </si>
+  <si>
+    <t>LY-tunnus</t>
+  </si>
+  <si>
+    <t>Data Universal Numbering System (D-U-N-S Number)</t>
+  </si>
+  <si>
+    <t>Global Location Number</t>
+  </si>
+  <si>
+    <t>DANISH CHAMBER OF COMMERCE Scheme</t>
+  </si>
+  <si>
+    <t>Vereniging van Kamers van Koophandel en Fabrieken in Nederland (Association of
+Chambers of Commerce and Industry in the Netherlands), Scheme</t>
+  </si>
+  <si>
+    <t>Vereniging van Kamers van Koophandel en Fabrieken in Nederland</t>
+  </si>
+  <si>
+    <t>Directorates of the European Commission</t>
+  </si>
+  <si>
+    <t>European Commission, Information Directorate, Data Transmission Service</t>
+  </si>
+  <si>
+    <t>SIA Object Identifiers</t>
+  </si>
+  <si>
+    <t>SECETI Object Identifiers</t>
+  </si>
+  <si>
+    <t>Organisatie Indentificatie Nummer (OIN)</t>
+  </si>
+  <si>
+    <t>Logius</t>
+  </si>
+  <si>
+    <t>Company code</t>
+  </si>
+  <si>
+    <t>Organisasjonsnummer</t>
+  </si>
+  <si>
+    <t>UBL.BE Party Identifier</t>
+  </si>
+  <si>
+    <t>lnfocomm Media Development Authority</t>
+  </si>
+  <si>
+    <t>Icelandic identifier</t>
+  </si>
+  <si>
+    <t>Hungarian VAT number</t>
+  </si>
+  <si>
+    <t>Belgian Crossroad Bank of Enterprise number</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1181,6 +1235,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1256,11 +1332,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1589,8 +1660,8 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1796875" defaultRowHeight="14.5"/>
@@ -1598,7 +1669,7 @@
     <col min="1" max="1" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1796875" style="6" bestFit="1" customWidth="1"/>
@@ -1612,70 +1683,73 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="101.5">
       <c r="A2" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G2" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="29">
@@ -1683,54 +1757,59 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>61</v>
+        <v>286</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="29">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>215</v>
-      </c>
       <c r="J4" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="130.5">
@@ -1738,29 +1817,32 @@
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>287</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="29">
@@ -1768,26 +1850,29 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>71</v>
+        <v>284</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G6" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="72.5">
@@ -1795,26 +1880,29 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>241</v>
+        <v>284</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G7" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1822,26 +1910,29 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>74</v>
+        <v>288</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G8" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="116">
@@ -1849,75 +1940,83 @@
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>289</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G9" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="29">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="58">
       <c r="A10" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="G10" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="58">
+    <row r="11" spans="1:12" ht="29">
       <c r="A11" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>276</v>
+        <v>284</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>339</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G11" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="130.5">
@@ -1925,26 +2024,29 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>289</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G12" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1952,97 +2054,106 @@
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>289</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="130.5">
       <c r="A14" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G14" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G14" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>239</v>
+        <v>288</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>236</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G15" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>226</v>
+        <v>290</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>343</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G16" s="6" t="b">
         <f>FALSE</f>
@@ -2051,100 +2162,112 @@
     </row>
     <row r="17" spans="1:11" ht="29">
       <c r="A17" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>251</v>
+        <v>292</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>248</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G17" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="G17" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>252</v>
-      </c>
       <c r="J17" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="58">
       <c r="A18" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G18" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>253</v>
-      </c>
       <c r="J18" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="43.5">
       <c r="A19" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>264</v>
+        <v>294</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>261</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G19" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="29">
       <c r="A20" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>272</v>
+        <v>295</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>347</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G20" s="6" t="b">
         <f>FALSE</f>
@@ -2153,19 +2276,22 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>37</v>
+        <v>296</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G21" s="6" t="b">
         <f>FALSE</f>
@@ -2177,26 +2303,29 @@
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E22" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>4</v>
       </c>
+      <c r="E22" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G22" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="29">
@@ -2204,23 +2333,26 @@
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E23" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>6</v>
       </c>
+      <c r="E23" s="18" t="s">
+        <v>6</v>
+      </c>
       <c r="F23" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G23" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="29">
@@ -2228,23 +2360,26 @@
         <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E24" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="E24" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G24" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2252,23 +2387,26 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E25" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>11</v>
       </c>
+      <c r="E25" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="F25" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G25" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2276,23 +2414,26 @@
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E26" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>13</v>
       </c>
+      <c r="E26" s="18" t="s">
+        <v>13</v>
+      </c>
       <c r="F26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G26" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="87">
@@ -2300,23 +2441,26 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E27" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>15</v>
       </c>
+      <c r="E27" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G27" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="29">
@@ -2324,44 +2468,48 @@
         <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E28" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G28" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="29">
+    <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="E29" s="17"/>
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G29" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K29" s="8">
         <v>990399123</v>
@@ -2372,20 +2520,26 @@
         <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G30" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="29">
@@ -2393,88 +2547,94 @@
         <v>25</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="17"/>
       <c r="F31" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G31" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="29">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="43.5">
+      <c r="A33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G32" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="29">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G33" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="29">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="17"/>
       <c r="F34" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G34" s="6" t="b">
         <f>FALSE</f>
@@ -2483,73 +2643,77 @@
     </row>
     <row r="35" spans="1:12" ht="29">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>298</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>107</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G35" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>37</v>
+        <v>296</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G36" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="43.5">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" s="17"/>
       <c r="F37" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G37" s="6" t="b">
         <f>FALSE</f>
@@ -2558,43 +2722,45 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="29">
-      <c r="A39" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="C39" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>109</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="17"/>
       <c r="F39" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G39" s="6" t="b">
         <f>FALSE</f>
@@ -2603,19 +2769,20 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>208</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="17"/>
       <c r="F40" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G40" s="6" t="b">
         <f>FALSE</f>
@@ -2624,19 +2791,20 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>175</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" s="17"/>
       <c r="F41" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G41" s="6" t="b">
         <f>FALSE</f>
@@ -2645,19 +2813,20 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>177</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="17"/>
       <c r="F42" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G42" s="6" t="b">
         <f>FALSE</f>
@@ -2666,19 +2835,20 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="17"/>
       <c r="F43" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G43" s="6" t="b">
         <f>FALSE</f>
@@ -2687,19 +2857,20 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>179</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="17"/>
       <c r="F44" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G44" s="6" t="b">
         <f>FALSE</f>
@@ -2708,19 +2879,20 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>180</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="E45" s="17"/>
       <c r="F45" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G45" s="6" t="b">
         <f>FALSE</f>
@@ -2729,19 +2901,20 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>181</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E46" s="17"/>
       <c r="F46" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G46" s="6" t="b">
         <f>FALSE</f>
@@ -2750,19 +2923,20 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>182</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E47" s="17"/>
       <c r="F47" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G47" s="6" t="b">
         <f>FALSE</f>
@@ -2771,19 +2945,20 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>183</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E48" s="17"/>
       <c r="F48" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G48" s="6" t="b">
         <f>FALSE</f>
@@ -2792,19 +2967,20 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>184</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" s="17"/>
       <c r="F49" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G49" s="6" t="b">
         <f>FALSE</f>
@@ -2813,19 +2989,20 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>185</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="E50" s="17"/>
       <c r="F50" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G50" s="6" t="b">
         <f>FALSE</f>
@@ -2834,19 +3011,20 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>205</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E51" s="17"/>
       <c r="F51" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G51" s="6" t="b">
         <f>FALSE</f>
@@ -2855,19 +3033,20 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>186</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" s="17"/>
       <c r="F52" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G52" s="6" t="b">
         <f>FALSE</f>
@@ -2876,19 +3055,20 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="17"/>
       <c r="F53" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G53" s="6" t="b">
         <f>FALSE</f>
@@ -2897,19 +3077,20 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>188</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E54" s="17"/>
       <c r="F54" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G54" s="6" t="b">
         <f>FALSE</f>
@@ -2918,19 +3099,20 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>189</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="E55" s="17"/>
       <c r="F55" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G55" s="6" t="b">
         <f>FALSE</f>
@@ -2939,40 +3121,42 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" s="17"/>
       <c r="F56" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G56" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" ht="29">
       <c r="A57" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>191</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E57" s="17"/>
       <c r="F57" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G57" s="6" t="b">
         <f>FALSE</f>
@@ -2981,19 +3165,20 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>192</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E58" s="17"/>
       <c r="F58" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G58" s="6" t="b">
         <f>FALSE</f>
@@ -3002,19 +3187,20 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>193</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="E59" s="17"/>
       <c r="F59" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G59" s="6" t="b">
         <f>FALSE</f>
@@ -3023,40 +3209,42 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>194</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E60" s="17"/>
       <c r="F60" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G60" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="29">
+    <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>195</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="17"/>
       <c r="F61" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G61" s="6" t="b">
         <f>FALSE</f>
@@ -3065,19 +3253,20 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>196</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E62" s="17"/>
       <c r="F62" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G62" s="6" t="b">
         <f>FALSE</f>
@@ -3086,19 +3275,20 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>197</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="17"/>
       <c r="F63" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G63" s="6" t="b">
         <f>FALSE</f>
@@ -3107,19 +3297,20 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>198</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E64" s="17"/>
       <c r="F64" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G64" s="6" t="b">
         <f>FALSE</f>
@@ -3128,19 +3319,20 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>199</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="17"/>
       <c r="F65" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G65" s="6" t="b">
         <f>FALSE</f>
@@ -3149,19 +3341,20 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>200</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E66" s="17"/>
       <c r="F66" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G66" s="6" t="b">
         <f>FALSE</f>
@@ -3170,19 +3363,20 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>201</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E67" s="17"/>
       <c r="F67" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G67" s="6" t="b">
         <f>FALSE</f>
@@ -3191,19 +3385,20 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E68" s="17"/>
       <c r="F68" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G68" s="6" t="b">
         <f>FALSE</f>
@@ -3212,40 +3407,44 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>202</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="E69" s="17"/>
       <c r="F69" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G69" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" ht="29">
       <c r="A70" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>203</v>
+        <v>326</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>230</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G70" s="6" t="b">
         <f>FALSE</f>
@@ -3254,19 +3453,20 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="E71" s="17"/>
+      <c r="F71" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="G71" s="6" t="b">
         <f>FALSE</f>
@@ -3275,19 +3475,20 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="E72" s="17"/>
       <c r="F72" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G72" s="6" t="b">
         <f>FALSE</f>
@@ -3296,46 +3497,46 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="F73" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G73" s="6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>237</v>
+        <v>286</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G74" s="6" t="b">
         <f>FALSE</f>
@@ -3344,43 +3545,43 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>233</v>
+        <v>294</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G75" s="6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>236</v>
+        <v>285</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G76" s="6" t="b">
         <f>FALSE</f>
@@ -3389,26 +3590,26 @@
     </row>
     <row r="77" spans="1:12" ht="43.5">
       <c r="A77" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="G77" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L77" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G77" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a typo in 0195 names
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Participant identifier schemes v5.xlsx
@@ -886,9 +886,6 @@
     <t>0195</t>
   </si>
   <si>
-    <t>Singaport Nationwide E-Invoice Framework</t>
-  </si>
-  <si>
     <t>SG:UEN</t>
   </si>
   <si>
@@ -1137,6 +1134,9 @@
   </si>
   <si>
     <t>Hungary VAT number</t>
+  </si>
+  <si>
+    <t>Singapore Nationwide E-Invoice Framework</t>
   </si>
 </sst>
 </file>
@@ -1672,8 +1672,8 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1796875" defaultRowHeight="14.5"/>
@@ -1701,10 +1701,10 @@
         <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>86</v>
@@ -1739,10 +1739,10 @@
         <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>63</v>
@@ -1772,10 +1772,10 @@
         <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>59</v>
@@ -1802,10 +1802,10 @@
         <v>211</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>215</v>
@@ -1832,10 +1832,10 @@
         <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>66</v>
@@ -1865,10 +1865,10 @@
         <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>69</v>
@@ -1895,10 +1895,10 @@
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>238</v>
@@ -1925,10 +1925,10 @@
         <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>72</v>
@@ -1955,7 +1955,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>73</v>
@@ -1985,13 +1985,13 @@
         <v>218</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>336</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>337</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>219</v>
@@ -2003,19 +2003,19 @@
     </row>
     <row r="11" spans="1:12" ht="29">
       <c r="A11" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>339</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>266</v>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>65</v>
@@ -2039,10 +2039,10 @@
         <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>75</v>
@@ -2069,10 +2069,10 @@
         <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>77</v>
@@ -2093,32 +2093,32 @@
     </row>
     <row r="14" spans="1:12" ht="130.5">
       <c r="A14" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="G14" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2129,7 +2129,7 @@
         <v>235</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>236</v>
@@ -2156,13 +2156,13 @@
         <v>240</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>342</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>343</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>246</v>
@@ -2180,10 +2180,10 @@
         <v>241</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>248</v>
@@ -2210,10 +2210,10 @@
         <v>242</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>247</v>
@@ -2240,10 +2240,10 @@
         <v>260</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>261</v>
@@ -2264,19 +2264,19 @@
     </row>
     <row r="20" spans="1:11" ht="29">
       <c r="A20" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>268</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>269</v>
+        <v>294</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>352</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>266</v>
@@ -2294,10 +2294,10 @@
         <v>265</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>35</v>
@@ -2318,7 +2318,7 @@
         <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>4</v>
@@ -2348,7 +2348,7 @@
         <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>6</v>
@@ -2375,7 +2375,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>9</v>
@@ -2402,7 +2402,7 @@
         <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>11</v>
@@ -2429,7 +2429,7 @@
         <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>13</v>
@@ -2454,7 +2454,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>15</v>
@@ -2481,7 +2481,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>20</v>
@@ -2505,7 +2505,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>20</v>
@@ -2533,10 +2533,10 @@
         <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>104</v>
@@ -2557,10 +2557,10 @@
         <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="2" t="s">
@@ -2574,7 +2574,7 @@
         <v>172</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2585,7 +2585,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>27</v>
@@ -2609,7 +2609,7 @@
         <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>30</v>
@@ -2636,7 +2636,7 @@
         <v>55</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>32</v>
@@ -2658,10 +2658,10 @@
         <v>56</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>107</v>
@@ -2685,7 +2685,7 @@
         <v>57</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>35</v>
@@ -2715,7 +2715,7 @@
         <v>96</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>95</v>
@@ -2737,7 +2737,7 @@
         <v>99</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>100</v>
@@ -2762,7 +2762,7 @@
         <v>102</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>107</v>
@@ -2784,7 +2784,7 @@
         <v>140</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>206</v>
@@ -2806,7 +2806,7 @@
         <v>141</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>173</v>
@@ -2828,7 +2828,7 @@
         <v>142</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>175</v>
@@ -2850,7 +2850,7 @@
         <v>143</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>174</v>
@@ -2872,7 +2872,7 @@
         <v>144</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D44" s="19" t="s">
         <v>177</v>
@@ -2894,7 +2894,7 @@
         <v>145</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D45" s="19" t="s">
         <v>178</v>
@@ -2916,7 +2916,7 @@
         <v>146</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>179</v>
@@ -2938,7 +2938,7 @@
         <v>147</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>180</v>
@@ -2960,7 +2960,7 @@
         <v>148</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>181</v>
@@ -2982,7 +2982,7 @@
         <v>149</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>182</v>
@@ -3004,7 +3004,7 @@
         <v>150</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>183</v>
@@ -3026,7 +3026,7 @@
         <v>151</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>203</v>
@@ -3048,7 +3048,7 @@
         <v>152</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>184</v>
@@ -3070,7 +3070,7 @@
         <v>153</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D53" s="19" t="s">
         <v>185</v>
@@ -3092,7 +3092,7 @@
         <v>154</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>186</v>
@@ -3114,7 +3114,7 @@
         <v>155</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>187</v>
@@ -3136,7 +3136,7 @@
         <v>208</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>188</v>
@@ -3158,7 +3158,7 @@
         <v>156</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>189</v>
@@ -3180,7 +3180,7 @@
         <v>157</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>190</v>
@@ -3202,7 +3202,7 @@
         <v>158</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>191</v>
@@ -3224,7 +3224,7 @@
         <v>159</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>192</v>
@@ -3246,7 +3246,7 @@
         <v>160</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>193</v>
@@ -3268,7 +3268,7 @@
         <v>161</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>194</v>
@@ -3290,7 +3290,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>195</v>
@@ -3312,7 +3312,7 @@
         <v>163</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>196</v>
@@ -3334,7 +3334,7 @@
         <v>164</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>197</v>
@@ -3356,7 +3356,7 @@
         <v>165</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>198</v>
@@ -3378,7 +3378,7 @@
         <v>166</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>199</v>
@@ -3400,7 +3400,7 @@
         <v>167</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>207</v>
@@ -3422,7 +3422,7 @@
         <v>168</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>200</v>
@@ -3444,7 +3444,7 @@
         <v>169</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>201</v>
@@ -3465,7 +3465,7 @@
         <v>170</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>202</v>
@@ -3487,7 +3487,7 @@
         <v>171</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>204</v>
@@ -3509,7 +3509,7 @@
         <v>220</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>223</v>
@@ -3536,7 +3536,7 @@
         <v>226</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>234</v>
@@ -3557,10 +3557,10 @@
         <v>229</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>230</v>
@@ -3584,7 +3584,7 @@
         <v>232</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>233</v>
@@ -3605,7 +3605,7 @@
         <v>256</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>257</v>

</xml_diff>